<commit_message>
paperr done, just needs an abstract and to have some latex issue resolved
</commit_message>
<xml_diff>
--- a/results/Summary.xlsx
+++ b/results/Summary.xlsx
@@ -211,10 +211,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000"/>
               <a:t>Single Process Single Node Speedup</a:t>
             </a:r>
           </a:p>
@@ -225,7 +225,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.090286697914607"/>
+          <c:y val="0.0835087719298245"/>
+          <c:w val="0.869527210132707"/>
+          <c:h val="0.759068794032325"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -723,11 +733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2089784984"/>
-        <c:axId val="-2127103224"/>
+        <c:axId val="1787082776"/>
+        <c:axId val="1787042712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2089784984"/>
+        <c:axId val="1787082776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -741,17 +751,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Number of</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:rPr lang="en-US" sz="1600" baseline="0"/>
                   <a:t> Threads</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1400"/>
+                <a:endParaRPr lang="en-US" sz="1600"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -759,8 +769,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.442077861264597"/>
-              <c:y val="0.954863038292852"/>
+              <c:x val="0.419824778509084"/>
+              <c:y val="0.951354330708662"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -773,12 +783,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127103224"/>
+        <c:crossAx val="1787042712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -786,10 +796,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127103224"/>
+        <c:axId val="1787042712"/>
         <c:scaling>
-          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
+          <c:min val="1.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -802,16 +812,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1600"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Speedup</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0089079320578669"/>
+              <c:y val="0.415004834921951"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -823,12 +840,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200"/>
+              <a:defRPr sz="1400"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2089784984"/>
+        <c:crossAx val="1787082776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -839,8 +856,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.231040602937927"/>
-          <c:y val="0.908934571289338"/>
+          <c:x val="0.240776340718189"/>
+          <c:y val="0.90367136344799"/>
           <c:w val="0.5398237941823"/>
           <c:h val="0.0437090758392043"/>
         </c:manualLayout>
@@ -873,8 +890,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
@@ -1229,7 +1246,7 @@
   <dimension ref="A2:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13:K34"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>